<commit_message>
Observações da avaliação 2o bimestre
</commit_message>
<xml_diff>
--- a/computadores-prova.xlsx
+++ b/computadores-prova.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0000000000000\Documents\git.repo\pm2025-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ProgMulti\Documents\git.repo\pm2025-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75275B3B-1D04-4044-BA9D-D172E2669F07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFCCAA7-8565-4F2B-A77B-5AC643E35D7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" activeTab="1" xr2:uid="{9E8B8019-333B-49E6-A78E-28E7B8C49CCE}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
   <si>
     <t>RA</t>
   </si>
@@ -84,12 +84,21 @@
   <si>
     <t>Computador</t>
   </si>
+  <si>
+    <t>Situação</t>
+  </si>
+  <si>
+    <t>Concluído</t>
+  </si>
+  <si>
+    <t>Não concluído</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +130,14 @@
       <color rgb="FF000000"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -161,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -185,6 +202,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -327,7 +345,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8327A63-CF23-45D9-93E0-2BE94C3EE45A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -381,9 +399,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -393,7 +411,7 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC304E76-0D12-4476-959E-B0B3DA76090F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -431,9 +449,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -443,7 +461,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1803BA78-2EA5-4EB3-9518-E1CC43D3A58B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -489,7 +507,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93857E38-4970-4CD4-9F39-053D09B84E4F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -543,9 +561,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -555,7 +573,7 @@
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0E83BCB-AD95-49F4-AC99-8C79968DDCC6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -593,9 +611,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -605,7 +623,7 @@
                   <a14:compatExt spid="_x0000_s1030"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2D54B77-FE00-45DA-8061-93A50246D363}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -651,7 +669,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54CED769-B526-4F36-864A-D7A43249D45B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -705,9 +723,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -717,7 +735,7 @@
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B575F05-DCCB-4612-AA2D-B97C2B33DB0D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -755,9 +773,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -767,7 +785,7 @@
                   <a14:compatExt spid="_x0000_s1033"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8579C773-45AA-4105-8F75-DC738CC51D32}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -813,7 +831,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{448EC9D7-B05F-4C98-B218-0741AB78D08C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -867,9 +885,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -879,7 +897,7 @@
                   <a14:compatExt spid="_x0000_s1035"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52DC901D-1D51-4153-BAF2-37EFC65BFE0F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -917,9 +935,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -929,7 +947,7 @@
                   <a14:compatExt spid="_x0000_s1036"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAA557D7-BB1D-49D9-BEEA-8CC31E36D175}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -975,7 +993,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFCDCE60-64F8-4A39-BEC0-AF8778609ABF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1029,9 +1047,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1041,7 +1059,7 @@
                   <a14:compatExt spid="_x0000_s1038"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB283AE0-F2D5-4870-A049-211F7D08AF84}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1079,9 +1097,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1091,7 +1109,7 @@
                   <a14:compatExt spid="_x0000_s1039"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6CA747A-ED4B-4EDC-9E3D-483FEC56625C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1137,7 +1155,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0737F8BC-FB99-403F-9145-FB7FA729041A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1191,9 +1209,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1203,7 +1221,7 @@
                   <a14:compatExt spid="_x0000_s1041"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CF4734F-32F0-454D-840A-9E60711D72DA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1241,9 +1259,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1253,7 +1271,7 @@
                   <a14:compatExt spid="_x0000_s1042"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15751323-98BB-4D35-9C7F-8A756AEADABB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1299,7 +1317,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02558F8A-B116-4F89-98B7-AAC25D2B0675}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1353,9 +1371,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1365,7 +1383,7 @@
                   <a14:compatExt spid="_x0000_s1044"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{545E237F-FEB9-4F76-BA26-7B414875C195}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1403,9 +1421,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1415,7 +1433,7 @@
                   <a14:compatExt spid="_x0000_s1045"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B588F726-02CD-4859-B908-F94BC1B4AA87}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1461,7 +1479,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40E14776-FCA9-483C-8ECF-78669EB13258}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1515,9 +1533,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1527,7 +1545,7 @@
                   <a14:compatExt spid="_x0000_s1047"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA0E69C5-AB64-47ED-B49C-9CE92934BB54}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1565,9 +1583,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1577,7 +1595,7 @@
                   <a14:compatExt spid="_x0000_s1048"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EAA5DE8-4807-4859-910A-F0C51F2656A6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1623,7 +1641,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D35AA75-077F-4C72-97C8-159C02DFF203}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1677,9 +1695,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1689,7 +1707,7 @@
                   <a14:compatExt spid="_x0000_s1050"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03295C15-8D6E-4072-A0F1-F712FCD50ED7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1727,9 +1745,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1739,7 +1757,7 @@
                   <a14:compatExt spid="_x0000_s1051"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFF34BCE-B580-4127-A6F2-32DAA8116109}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1785,7 +1803,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33C6A732-3B05-467B-8BDB-E51A0E76F59D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1839,9 +1857,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1851,7 +1869,7 @@
                   <a14:compatExt spid="_x0000_s1053"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02E32E66-AFA0-4976-8D5F-99EE34F53F4F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1889,9 +1907,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1901,7 +1919,7 @@
                   <a14:compatExt spid="_x0000_s1054"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F141FCD-B35A-4218-8638-E4B3F9383FE2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1947,7 +1965,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE2F730F-5D7A-42E8-8796-777B0663EF13}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2001,9 +2019,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2013,7 +2031,7 @@
                   <a14:compatExt spid="_x0000_s1056"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48728A05-26B8-4D56-B27E-7F663882A9E4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2051,9 +2069,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2063,7 +2081,7 @@
                   <a14:compatExt spid="_x0000_s1057"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4C51A9C-1A5E-4177-8E0C-E38A77E65086}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2109,7 +2127,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{700DCB7A-C313-465D-BEDA-60978272CEB3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2163,9 +2181,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2175,7 +2193,7 @@
                   <a14:compatExt spid="_x0000_s1059"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37BF45BC-2EE1-4F58-976D-0D53EBFB63F1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2213,9 +2231,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2225,7 +2243,7 @@
                   <a14:compatExt spid="_x0000_s1060"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F3A02C5-7FA4-4A30-B4BE-016D5564186E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2271,7 +2289,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24349609-59A8-4E19-956C-46E3BE9DD881}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2325,9 +2343,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2337,7 +2355,7 @@
                   <a14:compatExt spid="_x0000_s1062"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{977B6A00-0902-4AA1-964C-B7DCAD3FB580}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2375,9 +2393,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>203200</xdr:rowOff>
+          <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2387,7 +2405,7 @@
                   <a14:compatExt spid="_x0000_s1063"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7D0C438-4F0E-4ECB-9243-3ACC7A888BB7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2433,7 +2451,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1BA165B-A02B-4B7E-98FC-3492516F9552}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2783,9 +2801,9 @@
       <selection activeCell="C2" sqref="C2:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2800,7 +2818,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="22.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1781432412003</v>
       </c>
@@ -2811,7 +2829,7 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" ht="22.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1781432412004</v>
       </c>
@@ -2822,7 +2840,7 @@
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" ht="22.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1781432312005</v>
       </c>
@@ -2833,7 +2851,7 @@
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" ht="22.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1781432412005</v>
       </c>
@@ -2844,7 +2862,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" ht="22.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1781432412006</v>
       </c>
@@ -2855,7 +2873,7 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="33" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1781432412009</v>
       </c>
@@ -2866,7 +2884,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="22.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1781432412007</v>
       </c>
@@ -2877,7 +2895,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1781432412008</v>
       </c>
@@ -2888,7 +2906,7 @@
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="22.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>1781432412010</v>
       </c>
@@ -2899,7 +2917,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="22.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="33" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>1781432412011</v>
       </c>
@@ -2910,7 +2928,7 @@
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>1781432412016</v>
       </c>
@@ -2921,7 +2939,7 @@
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="22.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>1781432412017</v>
       </c>
@@ -2932,7 +2950,7 @@
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" ht="22.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>1781432412013</v>
       </c>
@@ -2943,7 +2961,7 @@
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>1781432412014</v>
       </c>
@@ -2962,7 +2980,632 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1063" r:id="rId4" name="Control 39">
+        <control shapeId="1026" r:id="rId4" name="Control 2">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1026" r:id="rId4" name="Control 2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1027" r:id="rId6" name="Control 3">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1027" r:id="rId6" name="Control 3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1029" r:id="rId7" name="Control 5">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1029" r:id="rId7" name="Control 5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1030" r:id="rId8" name="Control 6">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1030" r:id="rId8" name="Control 6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1032" r:id="rId9" name="Control 8">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1032" r:id="rId9" name="Control 8"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1033" r:id="rId10" name="Control 9">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1033" r:id="rId10" name="Control 9"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1035" r:id="rId11" name="Control 11">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1035" r:id="rId11" name="Control 11"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1036" r:id="rId12" name="Control 12">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1036" r:id="rId12" name="Control 12"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1038" r:id="rId13" name="Control 14">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1038" r:id="rId13" name="Control 14"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1039" r:id="rId14" name="Control 15">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1039" r:id="rId14" name="Control 15"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1041" r:id="rId15" name="Control 17">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1041" r:id="rId15" name="Control 17"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1042" r:id="rId16" name="Control 18">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1042" r:id="rId16" name="Control 18"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1044" r:id="rId17" name="Control 20">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1044" r:id="rId17" name="Control 20"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1045" r:id="rId18" name="Control 21">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1045" r:id="rId18" name="Control 21"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1047" r:id="rId19" name="Control 23">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1047" r:id="rId19" name="Control 23"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1048" r:id="rId20" name="Control 24">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1048" r:id="rId20" name="Control 24"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1050" r:id="rId21" name="Control 26">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1050" r:id="rId21" name="Control 26"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1051" r:id="rId22" name="Control 27">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1051" r:id="rId22" name="Control 27"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1053" r:id="rId23" name="Control 29">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1053" r:id="rId23" name="Control 29"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1054" r:id="rId24" name="Control 30">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1054" r:id="rId24" name="Control 30"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1056" r:id="rId25" name="Control 32">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1056" r:id="rId25" name="Control 32"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1057" r:id="rId26" name="Control 33">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1057" r:id="rId26" name="Control 33"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1059" r:id="rId27" name="Control 35">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1059" r:id="rId27" name="Control 35"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1060" r:id="rId28" name="Control 36">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1060" r:id="rId28" name="Control 36"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1062" r:id="rId29" name="Control 38">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>228600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1062" r:id="rId29" name="Control 38"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1063" r:id="rId30" name="Control 39">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
@@ -2973,641 +3616,16 @@
               </from>
               <to>
                 <xdr:col>4</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
+                <xdr:colOff>257175</xdr:colOff>
                 <xdr:row>13</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
+                <xdr:rowOff>228600</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1063" r:id="rId4" name="Control 39"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1062" r:id="rId6" name="Control 38">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1062" r:id="rId6" name="Control 38"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1060" r:id="rId7" name="Control 36">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1060" r:id="rId7" name="Control 36"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1059" r:id="rId8" name="Control 35">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1059" r:id="rId8" name="Control 35"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1057" r:id="rId9" name="Control 33">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>12700</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1057" r:id="rId9" name="Control 33"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1056" r:id="rId10" name="Control 32">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>12700</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1056" r:id="rId10" name="Control 32"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1054" r:id="rId11" name="Control 30">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1054" r:id="rId11" name="Control 30"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1053" r:id="rId12" name="Control 29">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1053" r:id="rId12" name="Control 29"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1051" r:id="rId13" name="Control 27">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1051" r:id="rId13" name="Control 27"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1050" r:id="rId14" name="Control 26">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1050" r:id="rId14" name="Control 26"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1048" r:id="rId15" name="Control 24">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1048" r:id="rId15" name="Control 24"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1047" r:id="rId16" name="Control 23">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1047" r:id="rId16" name="Control 23"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1045" r:id="rId17" name="Control 21">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1045" r:id="rId17" name="Control 21"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1044" r:id="rId18" name="Control 20">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1044" r:id="rId18" name="Control 20"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1042" r:id="rId19" name="Control 18">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1042" r:id="rId19" name="Control 18"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1041" r:id="rId20" name="Control 17">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1041" r:id="rId20" name="Control 17"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1039" r:id="rId21" name="Control 15">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1039" r:id="rId21" name="Control 15"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1038" r:id="rId22" name="Control 14">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1038" r:id="rId22" name="Control 14"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1036" r:id="rId23" name="Control 12">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1036" r:id="rId23" name="Control 12"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1035" r:id="rId24" name="Control 11">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1035" r:id="rId24" name="Control 11"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1033" r:id="rId25" name="Control 9">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1033" r:id="rId25" name="Control 9"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1032" r:id="rId26" name="Control 8">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1032" r:id="rId26" name="Control 8"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1030" r:id="rId27" name="Control 6">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1030" r:id="rId27" name="Control 6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId28" name="Control 5">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1029" r:id="rId28" name="Control 5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId29" name="Control 3">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1027" r:id="rId29" name="Control 3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId30" name="Control 2">
-          <controlPr defaultSize="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>203200</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1026" r:id="rId30" name="Control 2"/>
+        <control shapeId="1063" r:id="rId30" name="Control 39"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3616,135 +3634,183 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D04DB58-D969-4E13-9CBD-664953F8B034}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>18</v>
       </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3">
         <v>7</v>
       </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4">
         <v>14</v>
       </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6">
         <v>13</v>
       </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7">
         <v>16</v>
       </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8">
         <v>12</v>
       </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9">
         <v>11</v>
       </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11">
         <v>5</v>
       </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13">
         <v>8</v>
       </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14">
         <v>3</v>
       </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
       <c r="B15">
         <v>10</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>